<commit_message>
Revised majorly and ready for class
</commit_message>
<xml_diff>
--- a/LogarithmsIBM/AbsVsRelChangeStockSavings.xlsx
+++ b/LogarithmsIBM/AbsVsRelChangeStockSavings.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CalPoly\EC4990AINew\AIBookSlides\LogarithmsIBM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6222A41-8201-4238-B672-4D3876296436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{756A0E87-E88D-465B-B7D9-4920A7ABE86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AC75CDC8-0521-4287-8C00-1E4B4D9C1A47}"/>
+    <workbookView xWindow="45" yWindow="-21720" windowWidth="38640" windowHeight="21840" xr2:uid="{AC75CDC8-0521-4287-8C00-1E4B4D9C1A47}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Work Sheet" sheetId="2" r:id="rId1"/>
+    <sheet name="Completed Sheet" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
   <si>
     <t>t</t>
   </si>
@@ -48,9 +49,6 @@
   </si>
   <si>
     <t>Absolute Change per Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is an Example to Explain Relative Change and Logarithms  </t>
   </si>
   <si>
     <t>(the example  is not suited to compare Stock and Savings investments)</t>
@@ -76,6 +74,9 @@
   <si>
     <t>Savings Account Investment</t>
   </si>
+  <si>
+    <t xml:space="preserve">This is an Example to Explain Absolute Change vs. Relative Change and Logarithms  </t>
+  </si>
 </sst>
 </file>
 
@@ -83,9 +84,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="0.0000"/>
-    <numFmt numFmtId="173" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -119,7 +120,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,6 +139,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -437,7 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -474,10 +481,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -495,10 +502,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -513,10 +520,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -531,29 +538,68 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -889,416 +935,746 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9902A4C-B7EC-445A-90B4-DCD7677518CE}">
-  <dimension ref="A1:L15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A8479F8-B25E-4330-A848-BB0F51AD4686}">
+  <dimension ref="B1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="7.88671875" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.88671875" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" customWidth="1"/>
-    <col min="12" max="12" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" customWidth="1"/>
+    <col min="12" max="12" width="12.77734375" customWidth="1"/>
+    <col min="13" max="13" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="2:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+    </row>
+    <row r="2" spans="2:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="B2" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-    </row>
-    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-    </row>
-    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="4"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+    </row>
+    <row r="3" spans="2:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="F4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="6"/>
+      <c r="E4" s="4"/>
+      <c r="G4" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
-    </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="F5" s="6"/>
+      <c r="E5" s="4"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
-    </row>
-    <row r="6" spans="1:12" ht="90.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="2:13" ht="90.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="7"/>
+      <c r="G6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="H6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="J6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="13"/>
+      <c r="L6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="13"/>
-      <c r="K6" s="10" t="s">
+      <c r="M6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="15">
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="15">
         <v>0</v>
-      </c>
-      <c r="B7" s="16">
-        <v>100</v>
       </c>
       <c r="C7" s="16">
         <v>100</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="18">
+      <c r="D7" s="16">
+        <v>100</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="18">
         <v>0</v>
       </c>
-      <c r="G7" s="19">
+      <c r="H7" s="19">
         <v>100</v>
       </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="37">
-        <f>LN(G7)</f>
-        <v>4.6051701859880918</v>
-      </c>
-      <c r="L7" s="38"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="22">
+      <c r="I7" s="44"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="38"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="22">
         <v>1</v>
       </c>
-      <c r="B8" s="23">
+      <c r="C8" s="23">
         <v>100</v>
       </c>
-      <c r="C8" s="23">
-        <f>C7+4</f>
+      <c r="D8" s="23">
+        <f>D7+4</f>
         <v>104</v>
       </c>
-      <c r="D8" s="24">
-        <f>C8-C7</f>
-        <v>4</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="25">
+      <c r="E8" s="24"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="25">
         <v>1</v>
       </c>
-      <c r="G8" s="26">
-        <f>$G$7*(1+0.04)^F8</f>
+      <c r="H8" s="26">
+        <f>$H$7*(1+0.04)^G8</f>
         <v>104</v>
       </c>
-      <c r="H8" s="26">
-        <f>G8-G7</f>
-        <v>4</v>
-      </c>
-      <c r="I8" s="27">
-        <f>(G8-G7)/G7</f>
-        <v>0.04</v>
-      </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="37">
-        <f>LN(G8)</f>
-        <v>4.6443908991413725</v>
-      </c>
-      <c r="L8" s="35">
-        <f>K8-K7</f>
-        <v>3.9220713153280684E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="22">
+      <c r="I8" s="46"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="53"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="22">
         <v>2</v>
       </c>
-      <c r="B9" s="23">
+      <c r="C9" s="23">
         <v>100</v>
       </c>
-      <c r="C9" s="23">
-        <f t="shared" ref="C9:C12" si="0">C8+4</f>
+      <c r="D9" s="23">
+        <f t="shared" ref="D9:D12" si="0">D8+4</f>
         <v>108</v>
       </c>
-      <c r="D9" s="24">
-        <v>4</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="25">
+      <c r="E9" s="24"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="25">
         <v>2</v>
       </c>
-      <c r="G9" s="26">
-        <f t="shared" ref="G9:G12" si="1">$G$7*(1+0.04)^F9</f>
+      <c r="H9" s="26">
+        <f t="shared" ref="H9:H12" si="1">$H$7*(1+0.04)^G9</f>
         <v>108.16000000000001</v>
       </c>
-      <c r="H9" s="26">
-        <f t="shared" ref="H9:H12" si="2">G9-G8</f>
-        <v>4.1600000000000108</v>
-      </c>
-      <c r="I9" s="27">
-        <f t="shared" ref="I9:I12" si="3">(G9-G8)/G8</f>
-        <v>4.0000000000000105E-2</v>
-      </c>
-      <c r="J9" s="21"/>
-      <c r="K9" s="37">
-        <f t="shared" ref="K9:K12" si="4">LN(G9)</f>
-        <v>4.6836116122946541</v>
-      </c>
-      <c r="L9" s="35">
-        <f t="shared" ref="L9:L12" si="5">K9-K8</f>
-        <v>3.9220713153281572E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="22">
+      <c r="I9" s="46"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="53"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="22">
         <v>3</v>
       </c>
-      <c r="B10" s="23">
+      <c r="C10" s="23">
         <v>100</v>
       </c>
-      <c r="C10" s="23">
+      <c r="D10" s="23">
         <f t="shared" si="0"/>
         <v>112</v>
       </c>
-      <c r="D10" s="24">
-        <v>4</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="25">
+      <c r="E10" s="24"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="25">
         <v>3</v>
       </c>
-      <c r="G10" s="26">
+      <c r="H10" s="26">
         <f t="shared" si="1"/>
         <v>112.4864</v>
       </c>
-      <c r="H10" s="26">
-        <f t="shared" si="2"/>
-        <v>4.3263999999999925</v>
-      </c>
-      <c r="I10" s="27">
-        <f t="shared" si="3"/>
-        <v>3.9999999999999925E-2</v>
-      </c>
-      <c r="J10" s="21"/>
-      <c r="K10" s="37">
-        <f t="shared" si="4"/>
-        <v>4.7228323254479356</v>
-      </c>
-      <c r="L10" s="35">
-        <f t="shared" si="5"/>
-        <v>3.9220713153281572E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="22">
+      <c r="I10" s="46"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="53"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="22">
         <v>4</v>
       </c>
-      <c r="B11" s="23">
+      <c r="C11" s="23">
         <v>100</v>
       </c>
-      <c r="C11" s="23">
+      <c r="D11" s="23">
         <f t="shared" si="0"/>
         <v>116</v>
       </c>
-      <c r="D11" s="24">
+      <c r="E11" s="24"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="25">
         <v>4</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="25">
-        <v>4</v>
-      </c>
-      <c r="G11" s="26">
+      <c r="H11" s="26">
         <f t="shared" si="1"/>
         <v>116.98585600000003</v>
       </c>
-      <c r="H11" s="26">
-        <f t="shared" si="2"/>
-        <v>4.4994560000000234</v>
-      </c>
-      <c r="I11" s="27">
-        <f t="shared" si="3"/>
-        <v>4.0000000000000209E-2</v>
-      </c>
-      <c r="J11" s="21"/>
-      <c r="K11" s="37">
-        <f t="shared" si="4"/>
-        <v>4.7620530386012172</v>
-      </c>
-      <c r="L11" s="35">
-        <f t="shared" si="5"/>
-        <v>3.9220713153281572E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="28">
+      <c r="I11" s="46"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="53"/>
+    </row>
+    <row r="12" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="28">
         <v>5</v>
       </c>
-      <c r="B12" s="29">
+      <c r="C12" s="29">
         <v>100</v>
       </c>
-      <c r="C12" s="29">
+      <c r="D12" s="29">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="D12" s="30">
-        <v>4</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="31">
+      <c r="E12" s="30"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="31">
         <v>5</v>
       </c>
-      <c r="G12" s="32">
+      <c r="H12" s="32">
         <f t="shared" si="1"/>
         <v>121.66529024000003</v>
       </c>
-      <c r="H12" s="32">
-        <f t="shared" si="2"/>
-        <v>4.6794342400000062</v>
-      </c>
-      <c r="I12" s="33">
-        <f t="shared" si="3"/>
-        <v>4.0000000000000042E-2</v>
-      </c>
-      <c r="J12" s="34"/>
-      <c r="K12" s="39">
-        <f t="shared" si="4"/>
-        <v>4.8012737517544979</v>
-      </c>
-      <c r="L12" s="36">
-        <f t="shared" si="5"/>
-        <v>3.9220713153280684E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="54"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="F13" s="6"/>
+      <c r="E13" s="4"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="I13" s="41">
-        <f>SUM(I8:I12)</f>
-        <v>0.20000000000000026</v>
-      </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="L13" s="40">
-        <f>SUM(L8:L12)</f>
-        <v>0.19610356576640608</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="J13" s="50"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="M13" s="43"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="F14" s="6"/>
+      <c r="E14" s="4"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="F15" s="6"/>
+      <c r="E15" s="4"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" s="40">
-        <f>(G12-G7)/G7</f>
-        <v>0.21665290240000032</v>
-      </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="L15" s="40">
-        <f>K12-K7</f>
-        <v>0.19610356576640608</v>
-      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="40"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B2:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9902A4C-B7EC-445A-90B4-DCD7677518CE}">
+  <dimension ref="B1:M15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="7.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" customWidth="1"/>
+    <col min="12" max="12" width="12.77734375" customWidth="1"/>
+    <col min="13" max="13" width="15.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+    </row>
+    <row r="2" spans="2:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="B2" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+    </row>
+    <row r="3" spans="2:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="G4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="2:13" ht="90.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="13"/>
+      <c r="L6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="15">
+        <v>0</v>
+      </c>
+      <c r="C7" s="16">
+        <v>100</v>
+      </c>
+      <c r="D7" s="16">
+        <v>100</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="18">
+        <v>0</v>
+      </c>
+      <c r="H7" s="19">
+        <v>100</v>
+      </c>
+      <c r="I7" s="19"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="37">
+        <f>LN(H7)</f>
+        <v>4.6051701859880918</v>
+      </c>
+      <c r="M7" s="38"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="22">
+        <v>1</v>
+      </c>
+      <c r="C8" s="23">
+        <v>100</v>
+      </c>
+      <c r="D8" s="23">
+        <f>D7+4</f>
+        <v>104</v>
+      </c>
+      <c r="E8" s="24">
+        <f>D8-D7</f>
+        <v>4</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="25">
+        <v>1</v>
+      </c>
+      <c r="H8" s="26">
+        <f>$H$7*(1+0.04)^G8</f>
+        <v>104</v>
+      </c>
+      <c r="I8" s="26">
+        <f>H8-H7</f>
+        <v>4</v>
+      </c>
+      <c r="J8" s="27">
+        <f>(H8-H7)/H7</f>
+        <v>0.04</v>
+      </c>
+      <c r="K8" s="21"/>
+      <c r="L8" s="37">
+        <f>LN(H8)</f>
+        <v>4.6443908991413725</v>
+      </c>
+      <c r="M8" s="35">
+        <f>L8-L7</f>
+        <v>3.9220713153280684E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="22">
+        <v>2</v>
+      </c>
+      <c r="C9" s="23">
+        <v>100</v>
+      </c>
+      <c r="D9" s="23">
+        <f t="shared" ref="D9:D12" si="0">D8+4</f>
+        <v>108</v>
+      </c>
+      <c r="E9" s="24">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="25">
+        <v>2</v>
+      </c>
+      <c r="H9" s="26">
+        <f t="shared" ref="H9:H12" si="1">$H$7*(1+0.04)^G9</f>
+        <v>108.16000000000001</v>
+      </c>
+      <c r="I9" s="26">
+        <f t="shared" ref="I9:I12" si="2">H9-H8</f>
+        <v>4.1600000000000108</v>
+      </c>
+      <c r="J9" s="27">
+        <f t="shared" ref="J9:J12" si="3">(H9-H8)/H8</f>
+        <v>4.0000000000000105E-2</v>
+      </c>
+      <c r="K9" s="21"/>
+      <c r="L9" s="37">
+        <f t="shared" ref="L9:L12" si="4">LN(H9)</f>
+        <v>4.6836116122946541</v>
+      </c>
+      <c r="M9" s="35">
+        <f t="shared" ref="M9:M12" si="5">L9-L8</f>
+        <v>3.9220713153281572E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="22">
+        <v>3</v>
+      </c>
+      <c r="C10" s="23">
+        <v>100</v>
+      </c>
+      <c r="D10" s="23">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="E10" s="24">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="25">
+        <v>3</v>
+      </c>
+      <c r="H10" s="26">
+        <f t="shared" si="1"/>
+        <v>112.4864</v>
+      </c>
+      <c r="I10" s="26">
+        <f t="shared" si="2"/>
+        <v>4.3263999999999925</v>
+      </c>
+      <c r="J10" s="27">
+        <f t="shared" si="3"/>
+        <v>3.9999999999999925E-2</v>
+      </c>
+      <c r="K10" s="21"/>
+      <c r="L10" s="37">
+        <f t="shared" si="4"/>
+        <v>4.7228323254479356</v>
+      </c>
+      <c r="M10" s="35">
+        <f t="shared" si="5"/>
+        <v>3.9220713153281572E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="22">
+        <v>4</v>
+      </c>
+      <c r="C11" s="23">
+        <v>100</v>
+      </c>
+      <c r="D11" s="23">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+      <c r="E11" s="24">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="25">
+        <v>4</v>
+      </c>
+      <c r="H11" s="26">
+        <f t="shared" si="1"/>
+        <v>116.98585600000003</v>
+      </c>
+      <c r="I11" s="26">
+        <f t="shared" si="2"/>
+        <v>4.4994560000000234</v>
+      </c>
+      <c r="J11" s="27">
+        <f t="shared" si="3"/>
+        <v>4.0000000000000209E-2</v>
+      </c>
+      <c r="K11" s="21"/>
+      <c r="L11" s="37">
+        <f t="shared" si="4"/>
+        <v>4.7620530386012172</v>
+      </c>
+      <c r="M11" s="35">
+        <f t="shared" si="5"/>
+        <v>3.9220713153281572E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="28">
+        <v>5</v>
+      </c>
+      <c r="C12" s="29">
+        <v>100</v>
+      </c>
+      <c r="D12" s="29">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="E12" s="30">
+        <v>4</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="31">
+        <v>5</v>
+      </c>
+      <c r="H12" s="32">
+        <f t="shared" si="1"/>
+        <v>121.66529024000003</v>
+      </c>
+      <c r="I12" s="32">
+        <f t="shared" si="2"/>
+        <v>4.6794342400000062</v>
+      </c>
+      <c r="J12" s="33">
+        <f t="shared" si="3"/>
+        <v>4.0000000000000042E-2</v>
+      </c>
+      <c r="K12" s="34"/>
+      <c r="L12" s="39">
+        <f t="shared" si="4"/>
+        <v>4.8012737517544979</v>
+      </c>
+      <c r="M12" s="36">
+        <f t="shared" si="5"/>
+        <v>3.9220713153280684E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="J13" s="42">
+        <f>SUM(J8:J12)</f>
+        <v>0.20000000000000026</v>
+      </c>
+      <c r="K13" s="6"/>
+      <c r="L13" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="M13" s="43">
+        <f>SUM(M8:M12)</f>
+        <v>0.19610356576640608</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="40">
+        <f>(H12-H7)/H7</f>
+        <v>0.21665290240000032</v>
+      </c>
+      <c r="K15" s="6"/>
+      <c r="L15" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15" s="40">
+        <f>L12-L7</f>
+        <v>0.19610356576640608</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>